<commit_message>
Added architecture subsections to the cfm.
</commit_message>
<xml_diff>
--- a/CrossReferenceMatrix.xlsx
+++ b/CrossReferenceMatrix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Academics\2nd year\se\Youtube clone\CSAICSABTeam007\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5AD8FC-1A11-4642-8861-B2CACFB3AB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766CE153-41E2-486F-A6BD-E2085ED25EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9102599A-3A96-4FFD-962A-5BD2117DEB19}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="74">
   <si>
     <t>Stakeholder</t>
   </si>
@@ -235,6 +235,27 @@
   </si>
   <si>
     <t>Architecture Topic</t>
+  </si>
+  <si>
+    <t>1.3.1</t>
+  </si>
+  <si>
+    <t>Creator Features</t>
+  </si>
+  <si>
+    <t>1.3.2</t>
+  </si>
+  <si>
+    <t>Viewer Features</t>
+  </si>
+  <si>
+    <t>1.3.3</t>
+  </si>
+  <si>
+    <t>Advertiser Features</t>
+  </si>
+  <si>
+    <t>Container Diagrams</t>
   </si>
 </sst>
 </file>
@@ -619,7 +640,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,6 +709,12 @@
       <c r="E2" t="s">
         <v>40</v>
       </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
       <c r="H2" t="s">
         <v>43</v>
       </c>
@@ -708,6 +735,12 @@
       <c r="E3" t="s">
         <v>30</v>
       </c>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
       <c r="H3" t="s">
         <v>49</v>
       </c>
@@ -728,6 +761,12 @@
       <c r="E4" t="s">
         <v>29</v>
       </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>70</v>
+      </c>
       <c r="H4" t="s">
         <v>46</v>
       </c>
@@ -748,6 +787,12 @@
       <c r="E5" t="s">
         <v>32</v>
       </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" t="s">
+        <v>70</v>
+      </c>
       <c r="H5" t="s">
         <v>42</v>
       </c>
@@ -768,6 +813,12 @@
       <c r="E6" t="s">
         <v>31</v>
       </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>70</v>
+      </c>
       <c r="H6" t="s">
         <v>51</v>
       </c>
@@ -791,6 +842,12 @@
       <c r="E8" t="s">
         <v>28</v>
       </c>
+      <c r="F8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" t="s">
+        <v>68</v>
+      </c>
       <c r="H8" t="s">
         <v>41</v>
       </c>
@@ -811,6 +868,12 @@
       <c r="E9" t="s">
         <v>33</v>
       </c>
+      <c r="F9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" t="s">
+        <v>68</v>
+      </c>
       <c r="H9" t="s">
         <v>53</v>
       </c>
@@ -831,6 +894,12 @@
       <c r="E10" t="s">
         <v>29</v>
       </c>
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" t="s">
+        <v>68</v>
+      </c>
       <c r="H10" t="s">
         <v>55</v>
       </c>
@@ -851,6 +920,12 @@
       <c r="E11" t="s">
         <v>32</v>
       </c>
+      <c r="F11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" t="s">
+        <v>68</v>
+      </c>
       <c r="H11" t="s">
         <v>42</v>
       </c>
@@ -874,6 +949,12 @@
       <c r="E13" t="s">
         <v>34</v>
       </c>
+      <c r="F13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" t="s">
+        <v>72</v>
+      </c>
       <c r="H13" t="s">
         <v>61</v>
       </c>
@@ -894,6 +975,12 @@
       <c r="E14" t="s">
         <v>33</v>
       </c>
+      <c r="F14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" t="s">
+        <v>72</v>
+      </c>
       <c r="H14" t="s">
         <v>59</v>
       </c>
@@ -914,6 +1001,12 @@
       <c r="E15" t="s">
         <v>35</v>
       </c>
+      <c r="F15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" t="s">
+        <v>72</v>
+      </c>
       <c r="H15" t="s">
         <v>57</v>
       </c>
@@ -937,6 +1030,12 @@
       <c r="E17" t="s">
         <v>39</v>
       </c>
+      <c r="F17">
+        <v>1.2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>73</v>
+      </c>
       <c r="H17">
         <v>7.2</v>
       </c>
@@ -957,6 +1056,12 @@
       <c r="E18" t="s">
         <v>37</v>
       </c>
+      <c r="F18">
+        <v>1.2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>73</v>
+      </c>
       <c r="H18">
         <v>7.4</v>
       </c>
@@ -977,6 +1082,12 @@
       <c r="E19" t="s">
         <v>36</v>
       </c>
+      <c r="F19">
+        <v>1.2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>73</v>
+      </c>
       <c r="H19">
         <v>7.1</v>
       </c>
@@ -997,6 +1108,12 @@
       <c r="E20" t="s">
         <v>38</v>
       </c>
+      <c r="F20">
+        <v>1.2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>73</v>
+      </c>
       <c r="H20">
         <v>7.5</v>
       </c>
@@ -1016,6 +1133,12 @@
       </c>
       <c r="E21" t="s">
         <v>39</v>
+      </c>
+      <c r="F21">
+        <v>1.2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>73</v>
       </c>
       <c r="H21">
         <v>7.3</v>

</xml_diff>